<commit_message>
2nd try hpo SR
</commit_message>
<xml_diff>
--- a/HPOErgebnisse.xlsx
+++ b/HPOErgebnisse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\Ergebnisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D5B7E2-9AE8-496F-93DE-80FF373308C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C78A5-3CF2-4841-A8B4-5F259B7E9F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
   </bookViews>
   <sheets>
     <sheet name="Parity" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -286,9 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -298,7 +298,35 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -312,15 +340,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -336,15 +368,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -360,15 +396,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -384,15 +424,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -408,15 +452,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -432,15 +480,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -456,15 +508,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -480,15 +536,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -504,15 +564,19 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -526,8 +590,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -535,13 +603,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -564,9 +625,16 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -596,7 +664,29 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -612,45 +702,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -666,19 +726,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -694,19 +750,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -722,19 +774,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -750,19 +798,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -778,19 +822,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -806,19 +846,15 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -834,21 +870,40 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -862,68 +917,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -972,39 +972,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:J20" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:J20" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:J20" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:K20" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:K20" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:K20" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1329,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24624115-2EA4-43F4-B7C3-9E45AC575B2C}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -1834,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7223BD-063A-4B3D-9902-0134A848554C}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="D2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1897,6 +1897,11 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>

</xml_diff>